<commit_message>
Adedd Some New Details Backlog Produit & Journal updated
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A2E58-DA9D-4A9A-B6B1-AA052445DB24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866E6704-8DD0-4D3B-93EE-19D669FDC42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Theme</t>
   </si>
   <si>
-    <t>Epic</t>
-  </si>
-  <si>
-    <t>User Stories</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>catérogie client</t>
   </si>
   <si>
-    <t>Ahmed / Mariem</t>
-  </si>
-  <si>
     <t>Offre</t>
   </si>
   <si>
@@ -71,12 +62,6 @@
   </si>
   <si>
     <t>Engagement contractuel</t>
-  </si>
-  <si>
-    <t>User Story ID</t>
-  </si>
-  <si>
-    <t>Assigné à</t>
   </si>
   <si>
     <t>Statut</t>
@@ -107,9 +92,6 @@
     <t>À faire</t>
   </si>
   <si>
-    <t>Semaine 2</t>
-  </si>
-  <si>
     <t>VC-US-2</t>
   </si>
   <si>
@@ -120,10 +102,6 @@
   </si>
   <si>
     <t>Critères d'offre HD, XDSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semaine 2
-</t>
   </si>
   <si>
     <t>VC-US-3</t>
@@ -158,9 +136,6 @@
  non engagé</t>
   </si>
   <si>
-    <t>Semaine 3</t>
-  </si>
-  <si>
     <t>PROJECT NUMBER</t>
   </si>
   <si>
@@ -189,6 +164,45 @@
   </si>
   <si>
     <t>Project Management Templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Jours </t>
+  </si>
+  <si>
+    <t>Regroupement d'Objectifs</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Critere D'acceptation</t>
+  </si>
+  <si>
+    <t>Déterminer la catégorie client en fonction des dépenses annuelles.</t>
+  </si>
+  <si>
+    <t>Vérifier que le débit du client correspond aux critères définis.</t>
+  </si>
+  <si>
+    <t>Valider que le client est dans la période d'engagement ou Non.</t>
+  </si>
+  <si>
+    <t>Proposer les offres en fonction du type de service sélectionné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Jours </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 Jours </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID  Du l'Item  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    Niveau Utilisateur</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -205,11 +219,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -284,6 +293,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -335,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -416,78 +433,208 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +853,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -720,52 +867,52 @@
     <col min="4" max="4" width="206" customWidth="1"/>
     <col min="5" max="5" width="58.42578125" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
-    <col min="7" max="7" width="54.5703125" customWidth="1"/>
-    <col min="8" max="8" width="52.85546875" customWidth="1"/>
-    <col min="9" max="9" width="43.7109375" customWidth="1"/>
-    <col min="10" max="10" width="44.28515625" customWidth="1"/>
-    <col min="11" max="11" width="47.85546875" customWidth="1"/>
-    <col min="12" max="12" width="46.7109375" customWidth="1"/>
-    <col min="13" max="28" width="14.42578125" hidden="1"/>
+    <col min="7" max="7" width="52.85546875" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" customWidth="1"/>
+    <col min="9" max="9" width="44.28515625" customWidth="1"/>
+    <col min="10" max="10" width="47.85546875" customWidth="1"/>
+    <col min="11" max="11" width="46.7109375" customWidth="1"/>
+    <col min="12" max="27" width="14.42578125" hidden="1"/>
+    <col min="29" max="29" width="34.85546875" customWidth="1"/>
+    <col min="30" max="30" width="57.28515625" customWidth="1"/>
+    <col min="31" max="31" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -781,46 +928,51 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
+      <c r="AB1" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="47" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="22">
-        <f>K:K/J:J</f>
+        <v>17</v>
+      </c>
+      <c r="H2" s="22">
+        <f>J:J/I:I</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="J2" s="24">
+      <c r="I2" s="24">
         <v>60</v>
       </c>
-      <c r="K2" s="12">
+      <c r="J2" s="12">
         <v>80</v>
       </c>
-      <c r="L2" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="K2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -836,44 +988,49 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
+      <c r="AB2" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="48" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="31"/>
       <c r="B3" s="13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="20">
-        <f>K:K/J:J</f>
+        <v>17</v>
+      </c>
+      <c r="H3" s="20">
+        <f>J:J/I:I</f>
         <v>1.5</v>
       </c>
-      <c r="J3" s="25">
+      <c r="I3" s="25">
         <v>40</v>
       </c>
-      <c r="K3" s="28">
+      <c r="J3" s="28">
         <v>60</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="K3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -889,44 +1046,49 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
+      <c r="AB3" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC3" s="34"/>
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="49" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="31"/>
       <c r="B4" s="14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="23">
-        <f>K:K/J:J</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="J4" s="26">
-        <v>30</v>
-      </c>
-      <c r="K4" s="29">
+        <v>17</v>
+      </c>
+      <c r="H4" s="23">
+        <f>J:J/I:I</f>
+        <v>0.8</v>
+      </c>
+      <c r="I4" s="26">
+        <v>50</v>
+      </c>
+      <c r="J4" s="29">
         <v>40</v>
       </c>
-      <c r="L4" s="29" t="s">
-        <v>28</v>
-      </c>
+      <c r="K4" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -942,44 +1104,49 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
+      <c r="AB4" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="45"/>
+      <c r="AE4" s="50" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="32"/>
       <c r="B5" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="21">
-        <f>K:K/J:J</f>
-        <v>1.2</v>
-      </c>
-      <c r="J5" s="27">
-        <v>50</v>
-      </c>
-      <c r="K5" s="15">
+        <v>17</v>
+      </c>
+      <c r="H5" s="21">
+        <f>J:J/I:I</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I5" s="27">
+        <v>70</v>
+      </c>
+      <c r="J5" s="15">
         <v>60</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>37</v>
-      </c>
+      <c r="K5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -995,21 +1162,29 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
+      <c r="AB5" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="36"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="51" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A5"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J5" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"10,20,30,40,50,60,70,80,90,100"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H5" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G5" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"À faire,En Cours ,Réalisé"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1034,7 +1209,7 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="6"/>
@@ -1064,7 +1239,7 @@
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="6"/>
@@ -1094,7 +1269,7 @@
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6"/>
@@ -1124,7 +1299,7 @@
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
@@ -2182,33 +2357,33 @@
   <sheetData>
     <row r="2" spans="1:26" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>

</xml_diff>

<commit_message>
updated Backlog Produit & Sprint Backlog with details
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866E6704-8DD0-4D3B-93EE-19D669FDC42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D052334-56A6-4954-BC7A-4135AB78E37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Theme</t>
   </si>
@@ -197,12 +197,6 @@
   </si>
   <si>
     <t xml:space="preserve">ID  Du l'Item  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    Niveau Utilisateur</t>
-  </si>
-  <si>
-    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -352,7 +346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -458,21 +452,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -529,22 +508,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -607,6 +575,19 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,25 +597,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,10 +815,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -875,10 +837,9 @@
     <col min="12" max="27" width="14.42578125" hidden="1"/>
     <col min="29" max="29" width="34.85546875" customWidth="1"/>
     <col min="30" max="30" width="57.28515625" customWidth="1"/>
-    <col min="31" max="31" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -928,17 +889,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-      <c r="AB1" s="33" t="s">
+      <c r="AB1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="42"/>
-      <c r="AE1" s="47" t="s">
-        <v>51</v>
-      </c>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="38"/>
     </row>
-    <row r="2" spans="1:31" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:30" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="43" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -988,17 +946,14 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
-      <c r="AB2" s="39" t="s">
+      <c r="AB2" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="48" t="s">
-        <v>52</v>
-      </c>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="39"/>
     </row>
-    <row r="3" spans="1:31" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="31"/>
+    <row r="3" spans="1:30" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="44"/>
       <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
@@ -1046,17 +1001,14 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
-      <c r="AB3" s="38" t="s">
+      <c r="AB3" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="AC3" s="34"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="49" t="s">
-        <v>52</v>
-      </c>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="40"/>
     </row>
-    <row r="4" spans="1:31" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="31"/>
+    <row r="4" spans="1:30" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="44"/>
       <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
@@ -1104,17 +1056,14 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
-      <c r="AB4" s="40" t="s">
+      <c r="AB4" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="50" t="s">
-        <v>52</v>
-      </c>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="41"/>
     </row>
-    <row r="5" spans="1:31" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="32"/>
+    <row r="5" spans="1:30" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="45"/>
       <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
@@ -1162,14 +1111,11 @@
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
-      <c r="AB5" s="41" t="s">
+      <c r="AB5" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="AC5" s="36"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="51" t="s">
-        <v>52</v>
-      </c>
+      <c r="AC5" s="32"/>
+      <c r="AD5" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Page 15 et 13 a modifie
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D052334-56A6-4954-BC7A-4135AB78E37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962A5BC2-3834-448B-B8B8-DAEE9F1C34ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Theme</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">ID  Du l'Item  </t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -815,10 +818,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG4" sqref="AG4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1116,6 +1119,11 @@
       </c>
       <c r="AC5" s="32"/>
       <c r="AD5" s="42"/>
+    </row>
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updated ppt / Updated Baclog Produit / Update Sprint Backlog / Update Dig de Calsse
Co-Authored-By: Nacib Mariem <67750731+Nacib1999@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
+++ b/Conception Du Projet/TOPNET-Backlog Produit scoring - Premier Sprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Topnet-B2C-Stage-\Conception Du Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962A5BC2-3834-448B-B8B8-DAEE9F1C34ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF178D0C-6363-4B2A-ABD3-D66DB78E6CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,9 +76,6 @@
     <t>Business Value</t>
   </si>
   <si>
-    <t>VC-US-1</t>
-  </si>
-  <si>
     <t>Définir les critères pour la catégorie client</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>À faire</t>
   </si>
   <si>
-    <t>VC-US-2</t>
-  </si>
-  <si>
     <t>Définir les critères d'offre pour évaluer la valeur commerciale</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
   </si>
   <si>
     <t>Critères d'offre HD, XDSL</t>
-  </si>
-  <si>
-    <t>VC-US-3</t>
   </si>
   <si>
     <t>Établir les critères de débit pour évaluer la valeur commerciale</t>
@@ -122,9 +113,6 @@
  4</t>
   </si>
   <si>
-    <t>VC-US-4</t>
-  </si>
-  <si>
     <t>Identifier les critères d'engagement contractuel pour la valeur commerciale</t>
   </si>
   <si>
@@ -200,6 +188,18 @@
   </si>
   <si>
     <t>=</t>
+  </si>
+  <si>
+    <t>VC-i-1</t>
+  </si>
+  <si>
+    <t>VC-I-2</t>
+  </si>
+  <si>
+    <t>VC-I-3</t>
+  </si>
+  <si>
+    <t>VC-I-4</t>
   </si>
 </sst>
 </file>
@@ -821,7 +821,7 @@
   <dimension ref="A1:AD12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -830,7 +830,7 @@
     <col min="2" max="2" width="63.140625" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" customWidth="1"/>
     <col min="4" max="4" width="206" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="5" max="5" width="234.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59" customWidth="1"/>
     <col min="7" max="7" width="52.85546875" customWidth="1"/>
     <col min="8" max="8" width="43.7109375" customWidth="1"/>
@@ -847,13 +847,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>1</v>
@@ -893,7 +893,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AC1" s="1"/>
       <c r="AD1" s="38"/>
@@ -906,19 +906,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>16</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>17</v>
       </c>
       <c r="H2" s="22">
         <f>J:J/I:I</f>
@@ -931,7 +931,7 @@
         <v>80</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -950,7 +950,7 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="35" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AC2" s="33"/>
       <c r="AD2" s="39"/>
@@ -961,19 +961,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="F3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>21</v>
-      </c>
       <c r="G3" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="20">
         <f>J:J/I:I</f>
@@ -986,7 +986,7 @@
         <v>60</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1005,7 +1005,7 @@
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AC3" s="30"/>
       <c r="AD3" s="40"/>
@@ -1016,19 +1016,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" s="23">
         <f>J:J/I:I</f>
@@ -1041,7 +1041,7 @@
         <v>40</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -1060,7 +1060,7 @@
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AC4" s="31"/>
       <c r="AD4" s="41"/>
@@ -1071,19 +1071,19 @@
         <v>8</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="21">
         <f>J:J/I:I</f>
@@ -1096,7 +1096,7 @@
         <v>60</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1115,14 +1115,14 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AC5" s="32"/>
       <c r="AD5" s="42"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1163,7 +1163,7 @@
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="6"/>
@@ -1193,7 +1193,7 @@
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="6"/>
@@ -1223,7 +1223,7 @@
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6"/>
@@ -1253,7 +1253,7 @@
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="6"/>
@@ -2311,33 +2311,33 @@
   <sheetData>
     <row r="2" spans="1:26" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>

</xml_diff>